<commit_message>
modified:   01_3641_012900_AuroraSA_Grupo13.sql 	modified:   02_ActualizarTC.ps1 	modified:   03_3641_012900_AuroraSA_Grupo13.sql 	modified:   EjecucionCompleta.bat 	modified:   EjecucionCompletaAux.bat 	modified:   Pendiente.txt 	modified:   Procedures/Masivos/InsertarMasivoProductos.sql 	modified:   TP_integrador_Archivos/Productos/Productos_importados.xlsx
</commit_message>
<xml_diff>
--- a/TP_integrador_Archivos/Productos/Productos_importados.xlsx
+++ b/TP_integrador_Archivos/Productos/Productos_importados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingunlamedu.sharepoint.com/sites/BasesdeDatosAplicada-Docentes/Documentos compartidos/Docentes/2024/2doCuatrimestre/TP Integrador-Preparacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\OneDrive\Documents\Facultad\Base de datos aplicada\TP-SQL\TP_integrador_Archivos\Productos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D7921F72-74B3-4967-9545-46DCABF5D0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5ED696-A505-4E35-ABC6-CDD5609E0C26}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FCB6F-308C-460F-865E-BFD557DC179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Productos" sheetId="1" r:id="rId1"/>
@@ -599,10 +599,10 @@
     <t>12 cajas</t>
   </si>
   <si>
-    <t>Categoría</t>
-  </si>
-  <si>
     <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Categoria</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -659,16 +659,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,9 +709,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -749,7 +749,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -855,7 +855,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -997,7 +997,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1008,20 +1008,20 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,10 +1029,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1041,7 +1041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>21.35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>17.45</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>31.23</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>123.79</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>25.89</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>263.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>19.45</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>7.45</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>21.05</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2589,15 +2589,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="940421aca186f6b6cf253ceb76bcb39c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4f5da10e60c2eff5832bc3c34d166e5" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -2808,6 +2799,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2819,14 +2819,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B30EC333-6298-453C-BEC7-866D3958AD4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E50442C8-C288-454B-850D-C9F62A5D9B5A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2845,6 +2837,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B30EC333-6298-453C-BEC7-866D3958AD4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DCAD4BC-00B4-4EB9-AF68-58F534CC4AB3}">
   <ds:schemaRefs>

</xml_diff>